<commit_message>
Ran with all files
</commit_message>
<xml_diff>
--- a/Summary_iterations.xlsx
+++ b/Summary_iterations.xlsx
@@ -161,10 +161,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
+      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -295,6 +295,67 @@
       <c r="I3" s="0" t="n">
         <v>128</v>
       </c>
+      <c r="J3" s="0" t="n">
+        <v>0.420731273459036</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0.000274601843117833</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>0.000115763326662435</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>56290.9380028253</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <f aca="false">SQRT(M3)</f>
+        <v>237.25711370331</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0.0176456439379044</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0.00011056729969491</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>6.35549375038965E-005</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>79247.7238495054</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <f aca="false">SQRT(M4)</f>
+        <v>281.50972247776</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>